<commit_message>
migrating mysql to mysql2 using sequelizer
</commit_message>
<xml_diff>
--- a/assets/upload.xlsx
+++ b/assets/upload.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\others\node\projects\online-competition\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\others\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631C7100-503B-4115-AFF3-610407CCF0F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618F4438-0B8F-4D0E-8A1E-F55193F256E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{73B67342-A1CE-4D3E-95B4-4884C4E6CDC6}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,18 +25,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>CN01</t>
-  </si>
-  <si>
-    <t>NETOWRKS</t>
-  </si>
-  <si>
-    <t>DS01</t>
-  </si>
-  <si>
-    <t>data structures</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>brandName</t>
+  </si>
+  <si>
+    <t>ourPrice</t>
+  </si>
+  <si>
+    <t>originalPrice</t>
+  </si>
+  <si>
+    <t>imageUrl1</t>
+  </si>
+  <si>
+    <t>imageUrl2</t>
+  </si>
+  <si>
+    <t>imageUrl3</t>
+  </si>
+  <si>
+    <t>redmi</t>
+  </si>
+  <si>
+    <t>head phone</t>
+  </si>
+  <si>
+    <t>earpod</t>
+  </si>
+  <si>
+    <t>bluetooth</t>
+  </si>
+  <si>
+    <t>samsunf</t>
+  </si>
+  <si>
+    <t>zebronics</t>
+  </si>
+  <si>
+    <t>https://sp.yimg.com/ib/th?id=OPA.yaqWrHAvuTncGA474C474&amp;o=5&amp;pid=21.1&amp;w=96&amp;h=96</t>
+  </si>
+  <si>
+    <t>originalUrl</t>
   </si>
 </sst>
 </file>
@@ -108,7 +141,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -120,7 +153,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -167,23 +200,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -219,23 +235,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -387,32 +386,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E1322F-B7D6-4D1E-A744-835D7ACABBE7}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="77" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.6640625" customWidth="1"/>
+    <col min="7" max="7" width="77" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="76.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>240</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>340</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>430</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>